<commit_message>
span 60 done in 3 jobs
</commit_message>
<xml_diff>
--- a/series_02/mpi_0/span_060/qsmf_output.xlsx
+++ b/series_02/mpi_0/span_060/qsmf_output.xlsx
@@ -398,7 +398,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I119"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1363,13 +1363,13 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34">
-        <v>-7</v>
+        <v>1</v>
       </c>
       <c r="B34">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C34">
-        <v>5.4061</v>
+        <v>4.2183</v>
       </c>
       <c r="D34">
         <v>60</v>
@@ -1392,13 +1392,13 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35">
-        <v>-6</v>
+        <v>2</v>
       </c>
       <c r="B35">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C35">
-        <v>6.1348</v>
+        <v>3.2191</v>
       </c>
       <c r="D35">
         <v>60</v>
@@ -1421,13 +1421,13 @@
     </row>
     <row r="36" spans="1:9">
       <c r="A36">
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="B36">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C36">
-        <v>7.9194</v>
+        <v>2.2645</v>
       </c>
       <c r="D36">
         <v>60</v>
@@ -1450,13 +1450,13 @@
     </row>
     <row r="37" spans="1:9">
       <c r="A37">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="B37">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C37">
-        <v>7.4727</v>
+        <v>0.08040599999999999</v>
       </c>
       <c r="D37">
         <v>60</v>
@@ -1479,13 +1479,13 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38">
-        <v>0</v>
+        <v>-7</v>
       </c>
       <c r="B38">
         <v>18</v>
       </c>
       <c r="C38">
-        <v>7.114</v>
+        <v>5.4061</v>
       </c>
       <c r="D38">
         <v>60</v>
@@ -1508,13 +1508,13 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39">
-        <v>1</v>
+        <v>-6</v>
       </c>
       <c r="B39">
         <v>18</v>
       </c>
       <c r="C39">
-        <v>5.7714</v>
+        <v>6.1348</v>
       </c>
       <c r="D39">
         <v>60</v>
@@ -1537,13 +1537,13 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40">
-        <v>2</v>
+        <v>-5</v>
       </c>
       <c r="B40">
         <v>18</v>
       </c>
       <c r="C40">
-        <v>3.9522</v>
+        <v>6.7679</v>
       </c>
       <c r="D40">
         <v>60</v>
@@ -1566,13 +1566,13 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41">
-        <v>3</v>
+        <v>-4</v>
       </c>
       <c r="B41">
         <v>18</v>
       </c>
       <c r="C41">
-        <v>2.7962</v>
+        <v>7.3124</v>
       </c>
       <c r="D41">
         <v>60</v>
@@ -1595,13 +1595,13 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42">
-        <v>4</v>
+        <v>-3</v>
       </c>
       <c r="B42">
         <v>18</v>
       </c>
       <c r="C42">
-        <v>0.98326</v>
+        <v>7.6755</v>
       </c>
       <c r="D42">
         <v>60</v>
@@ -1624,13 +1624,13 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43">
-        <v>-7</v>
+        <v>-2</v>
       </c>
       <c r="B43">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C43">
-        <v>5.2224</v>
+        <v>7.9194</v>
       </c>
       <c r="D43">
         <v>60</v>
@@ -1653,13 +1653,13 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44">
-        <v>-6</v>
+        <v>-1</v>
       </c>
       <c r="B44">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C44">
-        <v>5.9398</v>
+        <v>7.4727</v>
       </c>
       <c r="D44">
         <v>60</v>
@@ -1682,13 +1682,13 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45">
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="B45">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C45">
-        <v>7.6557</v>
+        <v>7.114</v>
       </c>
       <c r="D45">
         <v>60</v>
@@ -1711,13 +1711,13 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B46">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C46">
-        <v>3.9382</v>
+        <v>5.7714</v>
       </c>
       <c r="D46">
         <v>60</v>
@@ -1740,13 +1740,13 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B47">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C47">
-        <v>2.1191</v>
+        <v>3.9522</v>
       </c>
       <c r="D47">
         <v>60</v>
@@ -1769,13 +1769,13 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="B48">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C48">
-        <v>5.176</v>
+        <v>2.7962</v>
       </c>
       <c r="D48">
         <v>60</v>
@@ -1798,13 +1798,13 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49">
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="B49">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C49">
-        <v>5.7738</v>
+        <v>0.98326</v>
       </c>
       <c r="D49">
         <v>60</v>
@@ -1827,13 +1827,13 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B50">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C50">
-        <v>6.5183</v>
+        <v>5.2224</v>
       </c>
       <c r="D50">
         <v>60</v>
@@ -1856,13 +1856,13 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B51">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C51">
-        <v>7.0448</v>
+        <v>5.9398</v>
       </c>
       <c r="D51">
         <v>60</v>
@@ -1885,13 +1885,13 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="B52">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C52">
-        <v>7.5354</v>
+        <v>6.5637</v>
       </c>
       <c r="D52">
         <v>60</v>
@@ -1914,13 +1914,13 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="B53">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C53">
-        <v>7.816</v>
+        <v>7.2437</v>
       </c>
       <c r="D53">
         <v>60</v>
@@ -1943,13 +1943,13 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B54">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C54">
-        <v>7.7553</v>
+        <v>7.6557</v>
       </c>
       <c r="D54">
         <v>60</v>
@@ -1972,13 +1972,13 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="B55">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C55">
-        <v>7.5713</v>
+        <v>7.7875</v>
       </c>
       <c r="D55">
         <v>60</v>
@@ -2001,13 +2001,13 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B56">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C56">
-        <v>6.9593</v>
+        <v>7.7265</v>
       </c>
       <c r="D56">
         <v>60</v>
@@ -2030,13 +2030,13 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B57">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C57">
-        <v>5.9777</v>
+        <v>7.3157</v>
       </c>
       <c r="D57">
         <v>60</v>
@@ -2059,13 +2059,13 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B58">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C58">
-        <v>4.9941</v>
+        <v>6.7368</v>
       </c>
       <c r="D58">
         <v>60</v>
@@ -2088,13 +2088,13 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B59">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C59">
-        <v>2.6788</v>
+        <v>5.1046</v>
       </c>
       <c r="D59">
         <v>60</v>
@@ -2117,13 +2117,13 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="B60">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C60">
-        <v>4.988</v>
+        <v>3.9382</v>
       </c>
       <c r="D60">
         <v>60</v>
@@ -2146,13 +2146,13 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61">
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="B61">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C61">
-        <v>5.6586</v>
+        <v>2.1191</v>
       </c>
       <c r="D61">
         <v>60</v>
@@ -2175,13 +2175,13 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B62">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C62">
-        <v>6.1847</v>
+        <v>5.176</v>
       </c>
       <c r="D62">
         <v>60</v>
@@ -2204,13 +2204,13 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B63">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C63">
-        <v>6.8691</v>
+        <v>5.7738</v>
       </c>
       <c r="D63">
         <v>60</v>
@@ -2233,13 +2233,13 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="B64">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C64">
-        <v>7.4006</v>
+        <v>6.5183</v>
       </c>
       <c r="D64">
         <v>60</v>
@@ -2262,13 +2262,13 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="B65">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C65">
-        <v>7.7265</v>
+        <v>7.0448</v>
       </c>
       <c r="D65">
         <v>60</v>
@@ -2291,13 +2291,13 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B66">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C66">
-        <v>7.9058</v>
+        <v>7.5354</v>
       </c>
       <c r="D66">
         <v>60</v>
@@ -2320,13 +2320,13 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="B67">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C67">
-        <v>7.6066</v>
+        <v>7.816</v>
       </c>
       <c r="D67">
         <v>60</v>
@@ -2349,13 +2349,13 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B68">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C68">
-        <v>7.0544</v>
+        <v>7.7553</v>
       </c>
       <c r="D68">
         <v>60</v>
@@ -2378,13 +2378,13 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B69">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C69">
-        <v>5.4424</v>
+        <v>7.5713</v>
       </c>
       <c r="D69">
         <v>60</v>
@@ -2407,13 +2407,13 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B70">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C70">
-        <v>5.2328</v>
+        <v>6.9593</v>
       </c>
       <c r="D70">
         <v>60</v>
@@ -2436,13 +2436,13 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B71">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C71">
-        <v>2.2253</v>
+        <v>5.9777</v>
       </c>
       <c r="D71">
         <v>60</v>
@@ -2465,13 +2465,13 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="B72">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C72">
-        <v>4.9102</v>
+        <v>4.9941</v>
       </c>
       <c r="D72">
         <v>60</v>
@@ -2494,13 +2494,13 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73">
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="B73">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C73">
-        <v>5.5181</v>
+        <v>2.6788</v>
       </c>
       <c r="D73">
         <v>60</v>
@@ -2523,13 +2523,13 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B74">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C74">
-        <v>6.1269</v>
+        <v>4.988</v>
       </c>
       <c r="D74">
         <v>60</v>
@@ -2552,13 +2552,13 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B75">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C75">
-        <v>6.7209</v>
+        <v>5.6586</v>
       </c>
       <c r="D75">
         <v>60</v>
@@ -2581,13 +2581,13 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="B76">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C76">
-        <v>7.2649</v>
+        <v>6.1847</v>
       </c>
       <c r="D76">
         <v>60</v>
@@ -2610,13 +2610,13 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="B77">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C77">
-        <v>7.5838</v>
+        <v>6.8691</v>
       </c>
       <c r="D77">
         <v>60</v>
@@ -2639,13 +2639,13 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B78">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C78">
-        <v>7.6901</v>
+        <v>7.4006</v>
       </c>
       <c r="D78">
         <v>60</v>
@@ -2668,13 +2668,13 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="B79">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C79">
-        <v>7.6874</v>
+        <v>7.7265</v>
       </c>
       <c r="D79">
         <v>60</v>
@@ -2697,13 +2697,13 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B80">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C80">
-        <v>7.2681</v>
+        <v>7.9058</v>
       </c>
       <c r="D80">
         <v>60</v>
@@ -2726,13 +2726,13 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B81">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C81">
-        <v>5.8734</v>
+        <v>7.6066</v>
       </c>
       <c r="D81">
         <v>60</v>
@@ -2755,13 +2755,13 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B82">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C82">
-        <v>5.577999999999999</v>
+        <v>7.0544</v>
       </c>
       <c r="D82">
         <v>60</v>
@@ -2784,13 +2784,13 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B83">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C83">
-        <v>3.5557</v>
+        <v>5.4424</v>
       </c>
       <c r="D83">
         <v>60</v>
@@ -2813,13 +2813,13 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="B84">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C84">
-        <v>4.7554</v>
+        <v>5.2328</v>
       </c>
       <c r="D84">
         <v>60</v>
@@ -2842,13 +2842,13 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85">
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="B85">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C85">
-        <v>5.3068</v>
+        <v>2.2253</v>
       </c>
       <c r="D85">
         <v>60</v>
@@ -2871,13 +2871,13 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B86">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C86">
-        <v>6.035</v>
+        <v>4.9102</v>
       </c>
       <c r="D86">
         <v>60</v>
@@ -2900,13 +2900,13 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B87">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C87">
-        <v>6.5754</v>
+        <v>5.5181</v>
       </c>
       <c r="D87">
         <v>60</v>
@@ -2929,13 +2929,13 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="B88">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C88">
-        <v>7.0943</v>
+        <v>6.1269</v>
       </c>
       <c r="D88">
         <v>60</v>
@@ -2958,13 +2958,13 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="B89">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C89">
-        <v>7.499</v>
+        <v>6.7209</v>
       </c>
       <c r="D89">
         <v>60</v>
@@ -2987,13 +2987,13 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B90">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C90">
-        <v>7.6169</v>
+        <v>7.2649</v>
       </c>
       <c r="D90">
         <v>60</v>
@@ -3016,13 +3016,13 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="B91">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C91">
-        <v>7.5038</v>
+        <v>7.5838</v>
       </c>
       <c r="D91">
         <v>60</v>
@@ -3045,13 +3045,13 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B92">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C92">
-        <v>7.229</v>
+        <v>7.6901</v>
       </c>
       <c r="D92">
         <v>60</v>
@@ -3074,13 +3074,13 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B93">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C93">
-        <v>5.6217</v>
+        <v>7.6874</v>
       </c>
       <c r="D93">
         <v>60</v>
@@ -3103,13 +3103,13 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B94">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C94">
-        <v>5.2794</v>
+        <v>7.2681</v>
       </c>
       <c r="D94">
         <v>60</v>
@@ -3132,13 +3132,13 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B95">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C95">
-        <v>3.8022</v>
+        <v>5.8734</v>
       </c>
       <c r="D95">
         <v>60</v>
@@ -3161,13 +3161,13 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="B96">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C96">
-        <v>4.5935</v>
+        <v>5.577999999999999</v>
       </c>
       <c r="D96">
         <v>60</v>
@@ -3190,13 +3190,13 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97">
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="B97">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C97">
-        <v>5.2011</v>
+        <v>3.5557</v>
       </c>
       <c r="D97">
         <v>60</v>
@@ -3219,13 +3219,13 @@
     </row>
     <row r="98" spans="1:9">
       <c r="A98">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B98">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C98">
-        <v>5.8226</v>
+        <v>4.7554</v>
       </c>
       <c r="D98">
         <v>60</v>
@@ -3248,13 +3248,13 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B99">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C99">
-        <v>6.5321</v>
+        <v>5.3068</v>
       </c>
       <c r="D99">
         <v>60</v>
@@ -3277,13 +3277,13 @@
     </row>
     <row r="100" spans="1:9">
       <c r="A100">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="B100">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C100">
-        <v>6.9319</v>
+        <v>6.035</v>
       </c>
       <c r="D100">
         <v>60</v>
@@ -3306,13 +3306,13 @@
     </row>
     <row r="101" spans="1:9">
       <c r="A101">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="B101">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C101">
-        <v>7.3069</v>
+        <v>6.5754</v>
       </c>
       <c r="D101">
         <v>60</v>
@@ -3335,13 +3335,13 @@
     </row>
     <row r="102" spans="1:9">
       <c r="A102">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B102">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C102">
-        <v>7.5074</v>
+        <v>7.0943</v>
       </c>
       <c r="D102">
         <v>60</v>
@@ -3364,13 +3364,13 @@
     </row>
     <row r="103" spans="1:9">
       <c r="A103">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="B103">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C103">
-        <v>7.6323</v>
+        <v>7.499</v>
       </c>
       <c r="D103">
         <v>60</v>
@@ -3393,13 +3393,13 @@
     </row>
     <row r="104" spans="1:9">
       <c r="A104">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B104">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C104">
-        <v>7.3211</v>
+        <v>7.6169</v>
       </c>
       <c r="D104">
         <v>60</v>
@@ -3422,13 +3422,13 @@
     </row>
     <row r="105" spans="1:9">
       <c r="A105">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B105">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C105">
-        <v>6.7061</v>
+        <v>7.5038</v>
       </c>
       <c r="D105">
         <v>60</v>
@@ -3451,13 +3451,13 @@
     </row>
     <row r="106" spans="1:9">
       <c r="A106">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B106">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C106">
-        <v>5.8512</v>
+        <v>7.229</v>
       </c>
       <c r="D106">
         <v>60</v>
@@ -3480,13 +3480,13 @@
     </row>
     <row r="107" spans="1:9">
       <c r="A107">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B107">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C107">
-        <v>3.7773</v>
+        <v>5.6217</v>
       </c>
       <c r="D107">
         <v>60</v>
@@ -3509,13 +3509,13 @@
     </row>
     <row r="108" spans="1:9">
       <c r="A108">
-        <v>-7</v>
+        <v>3</v>
       </c>
       <c r="B108">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C108">
-        <v>4.5165</v>
+        <v>5.2794</v>
       </c>
       <c r="D108">
         <v>60</v>
@@ -3538,13 +3538,13 @@
     </row>
     <row r="109" spans="1:9">
       <c r="A109">
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="B109">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C109">
-        <v>5.0926</v>
+        <v>3.8022</v>
       </c>
       <c r="D109">
         <v>60</v>
@@ -3567,13 +3567,13 @@
     </row>
     <row r="110" spans="1:9">
       <c r="A110">
-        <v>-5</v>
+        <v>-7</v>
       </c>
       <c r="B110">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C110">
-        <v>5.6608</v>
+        <v>4.5935</v>
       </c>
       <c r="D110">
         <v>60</v>
@@ -3596,13 +3596,13 @@
     </row>
     <row r="111" spans="1:9">
       <c r="A111">
-        <v>-4</v>
+        <v>-6</v>
       </c>
       <c r="B111">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C111">
-        <v>6.2076</v>
+        <v>5.2011</v>
       </c>
       <c r="D111">
         <v>60</v>
@@ -3625,13 +3625,13 @@
     </row>
     <row r="112" spans="1:9">
       <c r="A112">
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="B112">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C112">
-        <v>6.7209</v>
+        <v>5.8226</v>
       </c>
       <c r="D112">
         <v>60</v>
@@ -3654,13 +3654,13 @@
     </row>
     <row r="113" spans="1:9">
       <c r="A113">
-        <v>-2</v>
+        <v>-4</v>
       </c>
       <c r="B113">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C113">
-        <v>7.1917</v>
+        <v>6.5321</v>
       </c>
       <c r="D113">
         <v>60</v>
@@ -3683,13 +3683,13 @@
     </row>
     <row r="114" spans="1:9">
       <c r="A114">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="B114">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C114">
-        <v>7.4763</v>
+        <v>6.9319</v>
       </c>
       <c r="D114">
         <v>60</v>
@@ -3712,13 +3712,13 @@
     </row>
     <row r="115" spans="1:9">
       <c r="A115">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="B115">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C115">
-        <v>7.511</v>
+        <v>7.3069</v>
       </c>
       <c r="D115">
         <v>60</v>
@@ -3741,13 +3741,13 @@
     </row>
     <row r="116" spans="1:9">
       <c r="A116">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B116">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C116">
-        <v>7.0747</v>
+        <v>7.5074</v>
       </c>
       <c r="D116">
         <v>60</v>
@@ -3770,13 +3770,13 @@
     </row>
     <row r="117" spans="1:9">
       <c r="A117">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B117">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C117">
-        <v>6.6929</v>
+        <v>7.6323</v>
       </c>
       <c r="D117">
         <v>60</v>
@@ -3799,13 +3799,13 @@
     </row>
     <row r="118" spans="1:9">
       <c r="A118">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B118">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C118">
-        <v>5.8297</v>
+        <v>7.3211</v>
       </c>
       <c r="D118">
         <v>60</v>
@@ -3828,30 +3828,436 @@
     </row>
     <row r="119" spans="1:9">
       <c r="A119">
+        <v>2</v>
+      </c>
+      <c r="B119">
+        <v>54</v>
+      </c>
+      <c r="C119">
+        <v>6.7061</v>
+      </c>
+      <c r="D119">
+        <v>60</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>250</v>
+      </c>
+      <c r="G119">
+        <v>112</v>
+      </c>
+      <c r="H119">
+        <v>0.16</v>
+      </c>
+      <c r="I119">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120">
+        <v>3</v>
+      </c>
+      <c r="B120">
+        <v>54</v>
+      </c>
+      <c r="C120">
+        <v>5.8512</v>
+      </c>
+      <c r="D120">
+        <v>60</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>250</v>
+      </c>
+      <c r="G120">
+        <v>112</v>
+      </c>
+      <c r="H120">
+        <v>0.16</v>
+      </c>
+      <c r="I120">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121">
         <v>4</v>
       </c>
-      <c r="B119">
-        <v>60</v>
-      </c>
-      <c r="C119">
+      <c r="B121">
+        <v>54</v>
+      </c>
+      <c r="C121">
+        <v>3.7773</v>
+      </c>
+      <c r="D121">
+        <v>60</v>
+      </c>
+      <c r="E121">
+        <v>0</v>
+      </c>
+      <c r="F121">
+        <v>250</v>
+      </c>
+      <c r="G121">
+        <v>112</v>
+      </c>
+      <c r="H121">
+        <v>0.16</v>
+      </c>
+      <c r="I121">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122">
+        <v>-7</v>
+      </c>
+      <c r="B122">
+        <v>60</v>
+      </c>
+      <c r="C122">
+        <v>4.5165</v>
+      </c>
+      <c r="D122">
+        <v>60</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>250</v>
+      </c>
+      <c r="G122">
+        <v>112</v>
+      </c>
+      <c r="H122">
+        <v>0.16</v>
+      </c>
+      <c r="I122">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123">
+        <v>-6</v>
+      </c>
+      <c r="B123">
+        <v>60</v>
+      </c>
+      <c r="C123">
+        <v>5.0926</v>
+      </c>
+      <c r="D123">
+        <v>60</v>
+      </c>
+      <c r="E123">
+        <v>0</v>
+      </c>
+      <c r="F123">
+        <v>250</v>
+      </c>
+      <c r="G123">
+        <v>112</v>
+      </c>
+      <c r="H123">
+        <v>0.16</v>
+      </c>
+      <c r="I123">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9">
+      <c r="A124">
+        <v>-5</v>
+      </c>
+      <c r="B124">
+        <v>60</v>
+      </c>
+      <c r="C124">
+        <v>5.6608</v>
+      </c>
+      <c r="D124">
+        <v>60</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>250</v>
+      </c>
+      <c r="G124">
+        <v>112</v>
+      </c>
+      <c r="H124">
+        <v>0.16</v>
+      </c>
+      <c r="I124">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9">
+      <c r="A125">
+        <v>-4</v>
+      </c>
+      <c r="B125">
+        <v>60</v>
+      </c>
+      <c r="C125">
+        <v>6.2076</v>
+      </c>
+      <c r="D125">
+        <v>60</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <v>250</v>
+      </c>
+      <c r="G125">
+        <v>112</v>
+      </c>
+      <c r="H125">
+        <v>0.16</v>
+      </c>
+      <c r="I125">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9">
+      <c r="A126">
+        <v>-3</v>
+      </c>
+      <c r="B126">
+        <v>60</v>
+      </c>
+      <c r="C126">
+        <v>6.7209</v>
+      </c>
+      <c r="D126">
+        <v>60</v>
+      </c>
+      <c r="E126">
+        <v>0</v>
+      </c>
+      <c r="F126">
+        <v>250</v>
+      </c>
+      <c r="G126">
+        <v>112</v>
+      </c>
+      <c r="H126">
+        <v>0.16</v>
+      </c>
+      <c r="I126">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9">
+      <c r="A127">
+        <v>-2</v>
+      </c>
+      <c r="B127">
+        <v>60</v>
+      </c>
+      <c r="C127">
+        <v>7.1917</v>
+      </c>
+      <c r="D127">
+        <v>60</v>
+      </c>
+      <c r="E127">
+        <v>0</v>
+      </c>
+      <c r="F127">
+        <v>250</v>
+      </c>
+      <c r="G127">
+        <v>112</v>
+      </c>
+      <c r="H127">
+        <v>0.16</v>
+      </c>
+      <c r="I127">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9">
+      <c r="A128">
+        <v>-1</v>
+      </c>
+      <c r="B128">
+        <v>60</v>
+      </c>
+      <c r="C128">
+        <v>7.4763</v>
+      </c>
+      <c r="D128">
+        <v>60</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>250</v>
+      </c>
+      <c r="G128">
+        <v>112</v>
+      </c>
+      <c r="H128">
+        <v>0.16</v>
+      </c>
+      <c r="I128">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9">
+      <c r="A129">
+        <v>0</v>
+      </c>
+      <c r="B129">
+        <v>60</v>
+      </c>
+      <c r="C129">
+        <v>7.511</v>
+      </c>
+      <c r="D129">
+        <v>60</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <v>250</v>
+      </c>
+      <c r="G129">
+        <v>112</v>
+      </c>
+      <c r="H129">
+        <v>0.16</v>
+      </c>
+      <c r="I129">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
+      <c r="A130">
+        <v>1</v>
+      </c>
+      <c r="B130">
+        <v>60</v>
+      </c>
+      <c r="C130">
+        <v>7.0747</v>
+      </c>
+      <c r="D130">
+        <v>60</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>250</v>
+      </c>
+      <c r="G130">
+        <v>112</v>
+      </c>
+      <c r="H130">
+        <v>0.16</v>
+      </c>
+      <c r="I130">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9">
+      <c r="A131">
+        <v>2</v>
+      </c>
+      <c r="B131">
+        <v>60</v>
+      </c>
+      <c r="C131">
+        <v>6.6929</v>
+      </c>
+      <c r="D131">
+        <v>60</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <v>250</v>
+      </c>
+      <c r="G131">
+        <v>112</v>
+      </c>
+      <c r="H131">
+        <v>0.16</v>
+      </c>
+      <c r="I131">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
+      <c r="A132">
+        <v>3</v>
+      </c>
+      <c r="B132">
+        <v>60</v>
+      </c>
+      <c r="C132">
+        <v>5.8297</v>
+      </c>
+      <c r="D132">
+        <v>60</v>
+      </c>
+      <c r="E132">
+        <v>0</v>
+      </c>
+      <c r="F132">
+        <v>250</v>
+      </c>
+      <c r="G132">
+        <v>112</v>
+      </c>
+      <c r="H132">
+        <v>0.16</v>
+      </c>
+      <c r="I132">
+        <v>0.158</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
+      <c r="A133">
+        <v>4</v>
+      </c>
+      <c r="B133">
+        <v>60</v>
+      </c>
+      <c r="C133">
         <v>4.3487</v>
       </c>
-      <c r="D119">
-        <v>60</v>
-      </c>
-      <c r="E119">
-        <v>0</v>
-      </c>
-      <c r="F119">
-        <v>250</v>
-      </c>
-      <c r="G119">
-        <v>112</v>
-      </c>
-      <c r="H119">
-        <v>0.16</v>
-      </c>
-      <c r="I119">
+      <c r="D133">
+        <v>60</v>
+      </c>
+      <c r="E133">
+        <v>0</v>
+      </c>
+      <c r="F133">
+        <v>250</v>
+      </c>
+      <c r="G133">
+        <v>112</v>
+      </c>
+      <c r="H133">
+        <v>0.16</v>
+      </c>
+      <c r="I133">
         <v>0.158</v>
       </c>
     </row>

</xml_diff>